<commit_message>
Change: Added a row
</commit_message>
<xml_diff>
--- a/Simple Test Excel.xlsx
+++ b/Simple Test Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmdusa-my.sharepoint.com/personal/nferrufino_bmdusa_com/Documents/Documents/vc test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76698186-1190-4077-9DE2-7D33FF16452B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{76698186-1190-4077-9DE2-7D33FF16452B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C5686E5-2002-47CA-A7B0-13B5C69ECC0D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EFCEC0C0-3A27-4B92-82B4-60C0BB99A339}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Letter</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C78A373-0B74-4B24-A2D3-194F51CF8335}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -442,6 +445,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>